<commit_message>
corrected a mistake for the csv file reading
</commit_message>
<xml_diff>
--- a/moodys_datahub/data/data_products.xlsx
+++ b/moodys_datahub/data/data_products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/kgp_lib_cbs_dk/Documents/Desktop/moody-s_datahub/moodys_datahub/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="11_4B0D37945B70D6289F9A3B11595ED87656CCA927" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F141C444-FC36-4E18-8AF8-DEC33361F394}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="11_4B0D37945B70D6289F9A3B11595ED87656CCA927" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BAC39EC-3681-487B-9768-11E5D52F81C4}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="4395" windowWidth="28800" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29490" yWindow="4425" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -865,7 +865,7 @@
   <dimension ref="A1:D150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>